<commit_message>
Adicionados valores para 641
</commit_message>
<xml_diff>
--- a/Gráficos.xlsx
+++ b/Gráficos.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>15 MB</t>
   </si>
   <si>
     <t>150 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.357393 </t>
   </si>
 </sst>
 </file>
@@ -384,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,20 +423,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="2">
-        <v>0.18167</v>
+        <v>0.254189</v>
       </c>
       <c r="C7" s="2">
-        <v>1.911808</v>
+        <v>2.117</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="2">
-        <v>0.31533299999999997</v>
-      </c>
-      <c r="H7" s="2">
-        <v>3.36653</v>
-      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
       <c r="K7" s="1">
         <v>1</v>
       </c>
@@ -457,8 +456,12 @@
       <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2">
+        <v>0.129997</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.074014</v>
+      </c>
       <c r="F8" s="1">
         <v>2</v>
       </c>
@@ -469,8 +472,12 @@
       <c r="A9" s="1">
         <v>4</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2">
+        <v>6.5333000000000002E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.558948</v>
+      </c>
       <c r="F9" s="1">
         <v>4</v>
       </c>
@@ -481,8 +488,12 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2">
+        <v>3.6775000000000002E-2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -493,8 +504,12 @@
       <c r="A11" s="1">
         <v>16</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2">
+        <v>3.1687E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.30189100000000002</v>
+      </c>
       <c r="F11" s="1">
         <v>16</v>
       </c>
@@ -505,8 +520,12 @@
       <c r="A12" s="1">
         <v>20</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>2.7754000000000001E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.241983</v>
+      </c>
       <c r="F12" s="1">
         <v>20</v>
       </c>
@@ -517,8 +536,12 @@
       <c r="A13" s="1">
         <v>28</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2">
+        <v>6.1818999999999999E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.26135199999999997</v>
+      </c>
       <c r="F13" s="1">
         <v>28</v>
       </c>
@@ -529,8 +552,12 @@
       <c r="A14" s="1">
         <v>32</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2">
+        <v>0.49224099999999998</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.1221099999999999</v>
+      </c>
       <c r="F14" s="1">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Adicionado coisas ao relatorio
</commit_message>
<xml_diff>
--- a/Gráficos.xlsx
+++ b/Gráficos.xlsx
@@ -470,7 +470,7 @@
                   <c:v>6.1818999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.49224099999999998</c:v>
+                  <c:v>0.29224099999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -580,11 +580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1468643104"/>
-        <c:axId val="1753490400"/>
+        <c:axId val="-1841683184"/>
+        <c:axId val="-1841684272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1468643104"/>
+        <c:axId val="-1841683184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -683,7 +683,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1753490400"/>
+        <c:crossAx val="-1841684272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -691,7 +691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1753490400"/>
+        <c:axId val="-1841684272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,7 +798,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1468643104"/>
+        <c:crossAx val="-1841683184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1036,7 +1036,7 @@
                   <c:v>2.9500000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7100000000000002E-3</c:v>
+                  <c:v>3.7100000000000002E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1328,11 +1328,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1753493120"/>
-        <c:axId val="1753493664"/>
+        <c:axId val="-1841678832"/>
+        <c:axId val="-1841679920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1753493120"/>
+        <c:axId val="-1841678832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1753493664"/>
+        <c:crossAx val="-1841679920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1439,7 +1439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1753493664"/>
+        <c:axId val="-1841679920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,7 +1546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1753493120"/>
+        <c:crossAx val="-1841678832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1860,7 +1860,7 @@
                   <c:v>2.9500000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7100000000000002E-3</c:v>
+                  <c:v>3.7100000000000002E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1876,11 +1876,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1753492032"/>
-        <c:axId val="1753495840"/>
+        <c:axId val="-1841681552"/>
+        <c:axId val="-1841684816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1753492032"/>
+        <c:axId val="-1841681552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,7 +1979,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1753495840"/>
+        <c:crossAx val="-1841684816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1987,7 +1987,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1753495840"/>
+        <c:axId val="-1841684816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2094,7 +2094,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1753492032"/>
+        <c:crossAx val="-1841681552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2424,11 +2424,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1759858496"/>
-        <c:axId val="1759851424"/>
+        <c:axId val="-1840103520"/>
+        <c:axId val="-1840095360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1759858496"/>
+        <c:axId val="-1840103520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2527,7 +2527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759851424"/>
+        <c:crossAx val="-1840095360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2535,7 +2535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1759851424"/>
+        <c:axId val="-1840095360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2642,7 +2642,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759858496"/>
+        <c:crossAx val="-1840103520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2886,7 +2886,7 @@
                   <c:v>6.1818999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.49224099999999998</c:v>
+                  <c:v>0.29224099999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2996,11 +2996,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1753197360"/>
-        <c:axId val="1753198992"/>
+        <c:axId val="-1840106784"/>
+        <c:axId val="-1840102976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1753197360"/>
+        <c:axId val="-1840106784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3099,7 +3099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1753198992"/>
+        <c:crossAx val="-1840102976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3107,7 +3107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1753198992"/>
+        <c:axId val="-1840102976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3214,7 +3214,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1753197360"/>
+        <c:crossAx val="-1840106784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3568,11 +3568,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1759849792"/>
-        <c:axId val="1759859040"/>
+        <c:axId val="-1840105152"/>
+        <c:axId val="-1840092640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1759849792"/>
+        <c:axId val="-1840105152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3671,7 +3671,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759859040"/>
+        <c:crossAx val="-1840092640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3679,7 +3679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1759859040"/>
+        <c:axId val="-1840092640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3786,7 +3786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759849792"/>
+        <c:crossAx val="-1840105152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7677,8 +7677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="R16" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8158,7 +8158,7 @@
         <v>5.8100000000000003E-4</v>
       </c>
       <c r="T11" s="2">
-        <v>3.7100000000000002E-3</v>
+        <v>3.7100000000000002E-4</v>
       </c>
       <c r="U11" s="5"/>
       <c r="V11" s="5">
@@ -8210,7 +8210,7 @@
         <v>20</v>
       </c>
       <c r="I12" s="2">
-        <v>3.7100000000000002E-3</v>
+        <v>3.7100000000000002E-4</v>
       </c>
       <c r="J12" s="4">
         <v>9.4200000000000002E-4</v>
@@ -8267,7 +8267,7 @@
         <v>32</v>
       </c>
       <c r="AA13" s="2">
-        <v>0.49224099999999998</v>
+        <v>0.29224099999999997</v>
       </c>
       <c r="AB13" s="2">
         <v>2.9144E-2</v>
@@ -8291,7 +8291,7 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="2">
-        <v>0.49224099999999998</v>
+        <v>0.29224099999999997</v>
       </c>
       <c r="E14" s="2">
         <v>1.1221099999999999</v>

</xml_diff>